<commit_message>
Arreglo de modelo de dominio para el Spa y tambien modificacion en el diagrama
</commit_message>
<xml_diff>
--- a/SpaOnline/ModeloDominio/SpaOnline - Muestreo Datos.xlsx
+++ b/SpaOnline/ModeloDominio/SpaOnline - Muestreo Datos.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DOO\DOO\SpaOnline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grchia-my.sharepoint.com/personal/jhonatan_gomez_wiga_io/Documents/Escritorio/UCO/DOO GIT/SpaOnline/ModeloDominio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12307A28-BAB6-4BBA-B4B2-3CC3CEB1A98B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="156" documentId="13_ncr:1_{12307A28-BAB6-4BBA-B4B2-3CC3CEB1A98B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52CCD94C-4E4B-4F95-9C2E-2F48FEBC0573}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
+    <workbookView minimized="1" xWindow="2625" yWindow="0" windowWidth="15375" windowHeight="7785" firstSheet="1" activeTab="1" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo de Dominio Anemico" sheetId="1" r:id="rId1"/>
     <sheet name="Objetos de dominio" sheetId="2" r:id="rId2"/>
     <sheet name="SpaOnline" sheetId="5" r:id="rId3"/>
-    <sheet name="Servicios" sheetId="3" r:id="rId4"/>
+    <sheet name="TipoIdentificador" sheetId="6" r:id="rId4"/>
+    <sheet name="Trabajador" sheetId="8" r:id="rId5"/>
+    <sheet name="Administrador" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,10 +43,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={63682DA4-32B2-49D1-8057-879F2F5F7E58}</author>
+    <author>tc={60797445-8A4A-414B-9AFD-2A93089F955D}</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{63682DA4-32B2-49D1-8057-879F2F5F7E58}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{60797445-8A4A-414B-9AFD-2A93089F955D}">
       <text>
         <t xml:space="preserve">[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -59,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
   <si>
     <t xml:space="preserve">Nombre </t>
   </si>
@@ -73,9 +75,6 @@
     <t>Contextro</t>
   </si>
   <si>
-    <t>Fabricante</t>
-  </si>
-  <si>
     <t>Propio</t>
   </si>
   <si>
@@ -88,26 +87,101 @@
     <t>Combinacion única</t>
   </si>
   <si>
-    <t>Producto</t>
-  </si>
-  <si>
     <t>SpaOnline</t>
   </si>
   <si>
-    <t>Servicio</t>
-  </si>
-  <si>
-    <t>Objeto de dominio que contiene la informacion de los servicios que ofrece el Spa</t>
-  </si>
-  <si>
     <t>Objeto de dominio que contiene la informacion del personal que tiene el Spa</t>
+  </si>
+  <si>
+    <t>Numero Identificacion</t>
+  </si>
+  <si>
+    <t>TipoIdentificacion</t>
+  </si>
+  <si>
+    <t>SpaManitas</t>
+  </si>
+  <si>
+    <t>NIT</t>
+  </si>
+  <si>
+    <t>RUT</t>
+  </si>
+  <si>
+    <t>NIF</t>
+  </si>
+  <si>
+    <t>RNE</t>
+  </si>
+  <si>
+    <t>RUC</t>
+  </si>
+  <si>
+    <t>SpaOriente</t>
+  </si>
+  <si>
+    <t>TipoIdentificador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objeto de domino que contiene la informacion de los tipos de identificacion tributarios </t>
+  </si>
+  <si>
+    <t>NombreCompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jhonatan Arley Gómez </t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>Cristian David Ospina Ospina</t>
+  </si>
+  <si>
+    <t>Luis Ospina</t>
+  </si>
+  <si>
+    <t>Jhonatan12353</t>
+  </si>
+  <si>
+    <t>Cristian123</t>
+  </si>
+  <si>
+    <t>LuisOs432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jhoana Andrea Gómez Gómez </t>
+  </si>
+  <si>
+    <t>Jhoanago13</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>Trabajador</t>
+  </si>
+  <si>
+    <t>Juan Pablo Rendon Gómez</t>
+  </si>
+  <si>
+    <t>JPR3214</t>
+  </si>
+  <si>
+    <t>Objeto de domino que contiene la informacion de los trabajadores de cada Spa</t>
+  </si>
+  <si>
+    <t>Objeto de dominio que contiene la informacion del administrador de la empresa</t>
+  </si>
+  <si>
+    <t>Numero identificación</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +191,20 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -171,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -190,6 +278,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,7 +674,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C1" dT="2024-03-08T22:51:07.46" personId="{0BAE6951-F575-4CDD-BDEF-18025241A735}" id="{63682DA4-32B2-49D1-8057-879F2F5F7E58}">
+  <threadedComment ref="C1" dT="2024-03-08T22:51:07.46" personId="{0BAE6951-F575-4CDD-BDEF-18025241A735}" id="{60797445-8A4A-414B-9AFD-2A93089F955D}">
     <text xml:space="preserve">Propio: Es parte del contexto actual
 Impropios: que no hacen parte del contexto
 </text>
@@ -607,22 +702,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D92343-C7F8-498A-9249-704487594109}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68" style="9" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -636,32 +731,61 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -672,65 +796,125 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952BDDC5-1485-4BC4-A31B-18839936F54D}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.140625" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="4" t="str">
-        <f>B2&amp;"-"&amp;C2</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1">
+        <v>900811919</v>
+      </c>
+      <c r="D2" s="1" t="str">
+        <f>TipoIdentificador!C3</f>
+        <v>NIT</v>
+      </c>
+      <c r="E2" s="1" t="str">
+        <f>Administrador!E2</f>
+        <v>Jhoana Andrea Gómez Gómez -Jhoanago13</v>
+      </c>
+      <c r="F2" s="11" t="str">
+        <f>Trabajador!E2&amp;"-"&amp;Trabajador!E3</f>
+        <v>Jhonatan Arley Gómez -Jhonatan12353-Cristian David Ospina Ospina-Cristian123</v>
+      </c>
+      <c r="G2" s="4" t="str">
+        <f>C2&amp;"-"&amp;D2&amp;"-"&amp;B2</f>
+        <v>900811919-NIT-SpaOnline</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="4" t="str">
-        <f t="shared" ref="D3:D4" si="0">B3&amp;"-"&amp;C3</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1">
+        <v>811912382</v>
+      </c>
+      <c r="D3" s="1" t="str">
+        <f>TipoIdentificador!C3</f>
+        <v>NIT</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <f>Administrador!E2</f>
+        <v>Jhoana Andrea Gómez Gómez -Jhoanago13</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f>Trabajador!E4</f>
+        <v>Luis Ospina-LuisOs432</v>
+      </c>
+      <c r="G3" s="4" t="str">
+        <f t="shared" ref="G3:G4" si="0">C3&amp;"-"&amp;D3&amp;"-"&amp;B3</f>
+        <v>811912382-NIT-SpaManitas</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="4" t="str">
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1">
+        <v>830411223</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f>TipoIdentificador!C3</f>
+        <v>NIT</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f>Administrador!E2</f>
+        <v>Jhoana Andrea Gómez Gómez -Jhoanago13</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f>Trabajador!E5</f>
+        <v>Juan Pablo Rendon Gómez-JPR3214</v>
+      </c>
+      <c r="G4" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>830411223-NIT-SpaOriente</v>
       </c>
     </row>
   </sheetData>
@@ -739,59 +923,252 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27757F1-FD83-4C60-A977-3E4A8F875641}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{121986A6-D44D-4CDF-A74A-1517A7A7562F}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="4">
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4" t="str">
         <f>B2</f>
-        <v>0</v>
+        <v>RUT</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="4">
-        <f t="shared" ref="C3:C4" si="0">B3</f>
-        <v>0</v>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4" t="str">
+        <f t="shared" ref="C3:C6" si="0">B3</f>
+        <v>NIT</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>RNE</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>RUC</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>NIF</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A0EA0F-C535-46B8-908C-285392149FF0}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="27.7109375" customWidth="1"/>
+    <col min="5" max="5" width="38.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1038419180</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <f>B2&amp;"-"&amp;D2</f>
+        <v>Jhonatan Arley Gómez -Jhonatan12353</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="4">
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1038419181</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="4" t="str">
+        <f t="shared" ref="E3:E5" si="0">B3&amp;"-"&amp;D3</f>
+        <v>Cristian David Ospina Ospina-Cristian123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1038419182</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>Luis Ospina-LuisOs432</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1038419183</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>Juan Pablo Rendon Gómez-JPR3214</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D1ED5A-B972-4A71-A4D5-C7E705C9EC46}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1036416237</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <f>B2&amp;"-"&amp;C2</f>
+        <v>Jhoana Andrea Gómez Gómez -Jhoanago13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>